<commit_message>
added build_compilation_v2 wit associated changes in aux
</commit_message>
<xml_diff>
--- a/vgp_database/Bitterroot_Dome_intrusions.xlsx
+++ b/vgp_database/Bitterroot_Dome_intrusions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="102">
   <si>
     <t>Name:</t>
   </si>
@@ -105,10 +105,10 @@
     <t>R1</t>
   </si>
   <si>
-    <t>R2.1</t>
+    <t>R2a</t>
   </si>
   <si>
-    <t>R2.2</t>
+    <t>R2b</t>
   </si>
   <si>
     <t>R3</t>
@@ -117,10 +117,10 @@
     <t>R4</t>
   </si>
   <si>
-    <t>R5.1</t>
+    <t>R5a</t>
   </si>
   <si>
-    <t>R5.2</t>
+    <t>R5b</t>
   </si>
   <si>
     <t>R6</t>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>rhyolite dike</t>
+  </si>
+  <si>
+    <t>AF-TH</t>
   </si>
   <si>
     <t>Results these Bitterroot intrusions are interpreted to have suffered a few degrees of vertical axis rotation (on the basis of comparisons with 'reference' directions of Diehl et al. (1983)), but less severe than those from Skalkaho intrusions.</t>
@@ -328,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -368,13 +371,8 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,12 +393,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
@@ -412,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -466,17 +458,10 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -499,6 +484,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
@@ -1056,22 +1044,40 @@
       <c r="Y5" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="20"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="21"/>
+      <c r="Z5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AA5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AB5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AC5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AD5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AE5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AF5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AG5" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AH5" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AI5" s="3" t="s">
         <v>46</v>
       </c>
       <c r="AJ5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AK5" s="22" t="s">
+      <c r="AK5" s="19" t="s">
         <v>48</v>
       </c>
       <c r="AL5" s="3" t="s">
@@ -1085,24 +1091,24 @@
       <c r="A6" s="12">
         <v>2.0</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="24">
+      <c r="E6" s="21">
         <v>8.0</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="21">
         <v>46.4</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="21">
         <v>69.1</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="21">
         <v>18.1</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="21">
         <v>13.4</v>
       </c>
       <c r="J6" s="14"/>
@@ -1137,22 +1143,40 @@
       <c r="Y6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="20"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="21"/>
-      <c r="AH6" s="21"/>
+      <c r="Z6" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AA6" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AB6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AC6" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AD6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AE6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AF6" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AG6" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AH6" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AI6" s="3" t="s">
         <v>46</v>
       </c>
       <c r="AJ6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AK6" s="22" t="s">
+      <c r="AK6" s="19" t="s">
         <v>51</v>
       </c>
       <c r="AL6" s="3"/>
@@ -1373,39 +1397,39 @@
       <c r="AQ9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="23">
         <v>46.7</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="23">
         <f t="shared" ref="D10:D14" si="1">360-114.6</f>
         <v>245.4</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="24">
         <v>4.0</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="24">
         <v>336.9</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="24">
         <v>65.7</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="23">
         <v>94.5</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="24">
         <v>9.5</v>
       </c>
       <c r="J10" s="14"/>
-      <c r="K10" s="27">
+      <c r="K10" s="24">
         <v>74.2</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="24">
         <v>169.6</v>
       </c>
       <c r="M10" s="14"/>
@@ -1437,9 +1461,15 @@
       <c r="Y10" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
+      <c r="Z10" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA10" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB10" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC10" s="14"/>
       <c r="AD10" s="17">
         <v>0.0</v>
@@ -1459,7 +1489,7 @@
         <v>47</v>
       </c>
       <c r="AK10" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL10" s="3" t="s">
         <v>49</v>
@@ -1468,39 +1498,39 @@
       <c r="AN10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="23">
         <v>46.7</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="23">
         <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="24">
         <v>4.0</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="24">
         <v>342.8</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="24">
         <v>66.9</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="23">
         <v>60.4</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="24">
         <v>11.9</v>
       </c>
       <c r="J11" s="14"/>
-      <c r="K11" s="27">
+      <c r="K11" s="24">
         <v>78.3</v>
       </c>
-      <c r="L11" s="27">
+      <c r="L11" s="24">
         <v>175.6</v>
       </c>
       <c r="M11" s="14"/>
@@ -1532,9 +1562,15 @@
       <c r="Y11" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
+      <c r="Z11" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB11" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC11" s="14"/>
       <c r="AD11" s="17">
         <v>0.0</v>
@@ -1554,7 +1590,7 @@
         <v>47</v>
       </c>
       <c r="AK11" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL11" s="3" t="s">
         <v>49</v>
@@ -1563,39 +1599,39 @@
       <c r="AN11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="23" t="s">
+      <c r="A12" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="23">
         <v>46.7</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="23">
         <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="24">
         <v>7.0</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="24">
         <v>324.8</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="24">
         <v>59.0</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="23">
         <v>256.8</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="24">
         <v>3.8</v>
       </c>
       <c r="J12" s="14"/>
-      <c r="K12" s="27">
+      <c r="K12" s="24">
         <v>63.8</v>
       </c>
-      <c r="L12" s="27">
+      <c r="L12" s="24">
         <v>153.3</v>
       </c>
       <c r="M12" s="14"/>
@@ -1627,9 +1663,15 @@
       <c r="Y12" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21"/>
+      <c r="Z12" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA12" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB12" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC12" s="14"/>
       <c r="AD12" s="17">
         <v>0.0</v>
@@ -1649,7 +1691,7 @@
         <v>47</v>
       </c>
       <c r="AK12" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL12" s="3" t="s">
         <v>49</v>
@@ -1658,39 +1700,39 @@
       <c r="AN12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="23" t="s">
+      <c r="A13" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="23">
         <v>46.7</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="23">
         <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="24">
         <v>5.0</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="24">
         <v>331.4</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="24">
         <v>59.2</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="23">
         <v>48.6</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="24">
         <v>11.1</v>
       </c>
       <c r="J13" s="14"/>
-      <c r="K13" s="27">
+      <c r="K13" s="24">
         <v>69.4</v>
       </c>
-      <c r="L13" s="27">
+      <c r="L13" s="24">
         <v>150.2</v>
       </c>
       <c r="M13" s="14"/>
@@ -1722,9 +1764,15 @@
       <c r="Y13" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
+      <c r="Z13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA13" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB13" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC13" s="14"/>
       <c r="AD13" s="17">
         <v>0.0</v>
@@ -1744,7 +1792,7 @@
         <v>47</v>
       </c>
       <c r="AK13" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL13" s="3" t="s">
         <v>49</v>
@@ -1753,39 +1801,39 @@
       <c r="AN13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="23">
         <v>46.7</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="23">
         <f t="shared" si="1"/>
         <v>245.4</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="24">
         <v>3.0</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="24">
         <v>327.1</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="24">
         <v>50.9</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="23">
         <v>144.3</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="24">
         <v>10.3</v>
       </c>
       <c r="J14" s="14"/>
-      <c r="K14" s="27">
+      <c r="K14" s="24">
         <v>60.7</v>
       </c>
-      <c r="L14" s="27">
+      <c r="L14" s="24">
         <v>136.3</v>
       </c>
       <c r="M14" s="14"/>
@@ -1817,9 +1865,15 @@
       <c r="Y14" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z14" s="21"/>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="21"/>
+      <c r="Z14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA14" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB14" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC14" s="14"/>
       <c r="AD14" s="17">
         <v>0.0</v>
@@ -1839,7 +1893,7 @@
         <v>47</v>
       </c>
       <c r="AK14" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL14" s="3" t="s">
         <v>49</v>
@@ -1848,39 +1902,39 @@
       <c r="AN14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="23">
         <v>46.1</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="23">
         <f t="shared" ref="D15:D18" si="2">360-115.2</f>
         <v>244.8</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="24">
         <v>2.0</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="24">
         <v>171.7</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="24">
         <v>-64.6</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="23">
         <v>50.5</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="24">
         <v>35.9</v>
       </c>
       <c r="J15" s="14"/>
-      <c r="K15" s="27">
+      <c r="K15" s="24">
         <v>-84.2</v>
       </c>
-      <c r="L15" s="27">
+      <c r="L15" s="24">
         <v>-17.6</v>
       </c>
       <c r="M15" s="14"/>
@@ -1912,16 +1966,22 @@
       <c r="Y15" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
+      <c r="Z15" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA15" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB15" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC15" s="14"/>
       <c r="AD15" s="17">
         <v>0.0</v>
       </c>
       <c r="AE15" s="14"/>
       <c r="AF15" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG15" s="16">
         <v>1.0</v>
@@ -1934,7 +1994,7 @@
         <v>47</v>
       </c>
       <c r="AK15" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL15" s="3" t="s">
         <v>49</v>
@@ -1943,16 +2003,16 @@
       <c r="AN15" s="3"/>
     </row>
     <row r="16">
-      <c r="A16" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="23" t="s">
+      <c r="A16" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="23">
         <v>46.1</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="23">
         <f t="shared" si="2"/>
         <v>244.8</v>
       </c>
@@ -2007,9 +2067,15 @@
       <c r="Y16" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z16" s="21"/>
-      <c r="AA16" s="21"/>
-      <c r="AB16" s="21"/>
+      <c r="Z16" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA16" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB16" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC16" s="14"/>
       <c r="AD16" s="17">
         <v>0.0</v>
@@ -2018,10 +2084,10 @@
       <c r="AF16" s="18">
         <v>1.0</v>
       </c>
-      <c r="AG16" s="28">
+      <c r="AG16" s="25">
         <v>0.0</v>
       </c>
-      <c r="AH16" s="28">
+      <c r="AH16" s="25">
         <v>12.0</v>
       </c>
       <c r="AI16" s="3" t="s">
@@ -2031,7 +2097,7 @@
         <v>47</v>
       </c>
       <c r="AK16" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL16" s="3" t="s">
         <v>49</v>
@@ -2040,16 +2106,16 @@
       <c r="AN16" s="3"/>
     </row>
     <row r="17">
-      <c r="A17" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="23" t="s">
+      <c r="A17" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="23">
         <v>46.1</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="23">
         <f t="shared" si="2"/>
         <v>244.8</v>
       </c>
@@ -2104,9 +2170,15 @@
       <c r="Y17" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z17" s="21"/>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
+      <c r="Z17" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA17" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB17" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC17" s="14"/>
       <c r="AD17" s="17">
         <v>0.0</v>
@@ -2115,10 +2187,10 @@
       <c r="AF17" s="18">
         <v>1.0</v>
       </c>
-      <c r="AG17" s="28">
+      <c r="AG17" s="25">
         <v>0.0</v>
       </c>
-      <c r="AH17" s="28">
+      <c r="AH17" s="25">
         <v>12.0</v>
       </c>
       <c r="AI17" s="3" t="s">
@@ -2128,7 +2200,7 @@
         <v>47</v>
       </c>
       <c r="AK17" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL17" s="3" t="s">
         <v>49</v>
@@ -2137,39 +2209,39 @@
       <c r="AN17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="23" t="s">
+      <c r="A18" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="23">
         <v>46.1</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="23">
         <f t="shared" si="2"/>
         <v>244.8</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="24">
         <v>3.0</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="24">
         <v>344.0</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="24">
         <v>71.4</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="23">
         <v>48.5</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="24">
         <v>17.9</v>
       </c>
       <c r="J18" s="14"/>
-      <c r="K18" s="29">
+      <c r="K18" s="26">
         <v>75.9</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="26">
         <v>-154.3</v>
       </c>
       <c r="M18" s="14"/>
@@ -2201,9 +2273,15 @@
       <c r="Y18" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="21"/>
-      <c r="AB18" s="21"/>
+      <c r="Z18" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA18" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB18" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC18" s="14"/>
       <c r="AD18" s="17">
         <v>0.0</v>
@@ -2223,7 +2301,7 @@
         <v>47</v>
       </c>
       <c r="AK18" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL18" s="3" t="s">
         <v>49</v>
@@ -2232,39 +2310,39 @@
       <c r="AN18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="23" t="s">
+      <c r="A19" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="23">
         <v>46.1</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="23">
         <f t="shared" ref="D19:D28" si="3">360-115.1</f>
         <v>244.9</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="24">
         <v>2.0</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="24">
         <v>328.1</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="24">
         <v>78.1</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="23">
         <v>30.0</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="24">
         <v>47.3</v>
       </c>
       <c r="J19" s="14"/>
-      <c r="K19" s="29">
+      <c r="K19" s="26">
         <v>63.2</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="26">
         <v>-142.2</v>
       </c>
       <c r="M19" s="14"/>
@@ -2296,16 +2374,22 @@
       <c r="Y19" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
-      <c r="AB19" s="21"/>
+      <c r="Z19" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA19" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB19" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC19" s="14"/>
       <c r="AD19" s="17">
         <v>0.0</v>
       </c>
       <c r="AE19" s="14"/>
       <c r="AF19" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AG19" s="16">
         <v>1.0</v>
@@ -2318,7 +2402,7 @@
         <v>47</v>
       </c>
       <c r="AK19" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL19" s="3" t="s">
         <v>49</v>
@@ -2327,37 +2411,37 @@
       <c r="AN19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="23">
         <v>46.1</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="24">
         <v>4.0</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="24">
         <v>268.3</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="24">
         <v>81.8</v>
       </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="27">
+      <c r="H20" s="27"/>
+      <c r="I20" s="24">
         <v>13.3</v>
       </c>
       <c r="J20" s="14"/>
-      <c r="K20" s="29">
+      <c r="K20" s="26">
         <v>43.3</v>
       </c>
-      <c r="L20" s="29">
+      <c r="L20" s="26">
         <v>-137.5</v>
       </c>
       <c r="M20" s="14"/>
@@ -2389,9 +2473,15 @@
       <c r="Y20" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
+      <c r="Z20" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA20" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB20" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC20" s="14"/>
       <c r="AD20" s="17">
         <v>0.0</v>
@@ -2400,10 +2490,10 @@
       <c r="AF20" s="18">
         <v>2.0</v>
       </c>
-      <c r="AG20" s="28">
+      <c r="AG20" s="25">
         <v>0.0</v>
       </c>
-      <c r="AH20" s="28">
+      <c r="AH20" s="25">
         <v>12.0</v>
       </c>
       <c r="AI20" s="3" t="s">
@@ -2413,7 +2503,7 @@
         <v>47</v>
       </c>
       <c r="AK20" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL20" s="3" t="s">
         <v>49</v>
@@ -2422,16 +2512,16 @@
       <c r="AN20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="23" t="s">
+      <c r="A21" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="23">
         <v>46.1</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
@@ -2486,9 +2576,15 @@
       <c r="Y21" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
-      <c r="AB21" s="21"/>
+      <c r="Z21" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA21" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB21" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC21" s="14"/>
       <c r="AD21" s="17">
         <v>0.0</v>
@@ -2497,10 +2593,10 @@
       <c r="AF21" s="18">
         <v>2.0</v>
       </c>
-      <c r="AG21" s="28">
+      <c r="AG21" s="25">
         <v>0.0</v>
       </c>
-      <c r="AH21" s="28">
+      <c r="AH21" s="25">
         <v>12.0</v>
       </c>
       <c r="AI21" s="3" t="s">
@@ -2510,7 +2606,7 @@
         <v>47</v>
       </c>
       <c r="AK21" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL21" s="3" t="s">
         <v>49</v>
@@ -2519,39 +2615,39 @@
       <c r="AN21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="23" t="s">
+      <c r="A22" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="23">
         <v>46.1</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="24">
         <v>2.0</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="24">
         <v>163.0</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="24">
         <v>-57.7</v>
       </c>
-      <c r="H22" s="26">
+      <c r="H22" s="23">
         <v>1362.9</v>
       </c>
-      <c r="I22" s="27">
+      <c r="I22" s="24">
         <v>6.8</v>
       </c>
       <c r="J22" s="14"/>
-      <c r="K22" s="29">
+      <c r="K22" s="26">
         <v>-75.5</v>
       </c>
-      <c r="L22" s="29">
+      <c r="L22" s="26">
         <v>-50.8</v>
       </c>
       <c r="M22" s="14"/>
@@ -2583,16 +2679,22 @@
       <c r="Y22" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
+      <c r="Z22" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA22" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB22" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC22" s="14"/>
       <c r="AD22" s="17">
         <v>0.0</v>
       </c>
       <c r="AE22" s="14"/>
       <c r="AF22" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AG22" s="16">
         <v>1.0</v>
@@ -2605,7 +2707,7 @@
         <v>47</v>
       </c>
       <c r="AK22" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL22" s="3" t="s">
         <v>49</v>
@@ -2614,39 +2716,39 @@
       <c r="AN22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="23" t="s">
+      <c r="A23" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="23">
         <v>46.1</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="24">
         <v>5.0</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="24">
         <v>160.1</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="24">
         <v>-57.7</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H23" s="23">
         <v>333.0</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="24">
         <v>4.2</v>
       </c>
       <c r="J23" s="14"/>
-      <c r="K23" s="29">
+      <c r="K23" s="26">
         <v>-73.4</v>
       </c>
-      <c r="L23" s="29">
+      <c r="L23" s="26">
         <v>-45.7</v>
       </c>
       <c r="M23" s="14"/>
@@ -2678,9 +2780,15 @@
       <c r="Y23" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z23" s="21"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="21"/>
+      <c r="Z23" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA23" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB23" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC23" s="14"/>
       <c r="AD23" s="17">
         <v>0.0</v>
@@ -2689,10 +2797,10 @@
       <c r="AF23" s="18">
         <v>3.0</v>
       </c>
-      <c r="AG23" s="28">
+      <c r="AG23" s="25">
         <v>0.0</v>
       </c>
-      <c r="AH23" s="28">
+      <c r="AH23" s="25">
         <v>12.0</v>
       </c>
       <c r="AI23" s="3" t="s">
@@ -2702,7 +2810,7 @@
         <v>47</v>
       </c>
       <c r="AK23" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL23" s="3" t="s">
         <v>49</v>
@@ -2711,39 +2819,39 @@
       <c r="AN23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="23" t="s">
+      <c r="A24" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="23">
         <v>46.1</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="24">
         <v>3.0</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="24">
         <v>165.9</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="24">
         <v>-57.6</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="23">
         <v>3905.3</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="24">
         <v>2.0</v>
       </c>
       <c r="J24" s="14"/>
-      <c r="K24" s="29">
+      <c r="K24" s="26">
         <v>-77.0</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L24" s="26">
         <v>-56.9</v>
       </c>
       <c r="M24" s="14"/>
@@ -2775,9 +2883,15 @@
       <c r="Y24" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z24" s="21"/>
-      <c r="AA24" s="21"/>
-      <c r="AB24" s="21"/>
+      <c r="Z24" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA24" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB24" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC24" s="14"/>
       <c r="AD24" s="17">
         <v>0.0</v>
@@ -2786,10 +2900,10 @@
       <c r="AF24" s="18">
         <v>3.0</v>
       </c>
-      <c r="AG24" s="28">
+      <c r="AG24" s="25">
         <v>0.0</v>
       </c>
-      <c r="AH24" s="28">
+      <c r="AH24" s="25">
         <v>12.0</v>
       </c>
       <c r="AI24" s="3" t="s">
@@ -2799,7 +2913,7 @@
         <v>47</v>
       </c>
       <c r="AK24" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL24" s="3" t="s">
         <v>49</v>
@@ -2808,39 +2922,39 @@
       <c r="AN24" s="3"/>
     </row>
     <row r="25">
-      <c r="A25" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="23" t="s">
+      <c r="A25" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="23">
         <v>46.1</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="24">
         <v>2.0</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="24">
         <v>120.3</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="24">
         <v>-66.9</v>
       </c>
-      <c r="H25" s="26">
+      <c r="H25" s="23">
         <v>40.4</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="24">
         <v>40.4</v>
       </c>
       <c r="J25" s="14"/>
-      <c r="K25" s="29">
+      <c r="K25" s="26">
         <v>-50.9</v>
       </c>
-      <c r="L25" s="29">
+      <c r="L25" s="26">
         <v>2.5</v>
       </c>
       <c r="M25" s="14"/>
@@ -2872,16 +2986,22 @@
       <c r="Y25" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z25" s="21"/>
-      <c r="AA25" s="21"/>
-      <c r="AB25" s="21"/>
+      <c r="Z25" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA25" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB25" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC25" s="14"/>
       <c r="AD25" s="17">
         <v>0.0</v>
       </c>
       <c r="AE25" s="14"/>
       <c r="AF25" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AG25" s="16">
         <v>1.0</v>
@@ -2894,7 +3014,7 @@
         <v>47</v>
       </c>
       <c r="AK25" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL25" s="3" t="s">
         <v>49</v>
@@ -2903,38 +3023,38 @@
       <c r="AN25" s="3"/>
     </row>
     <row r="26">
-      <c r="A26" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" s="23" t="s">
+      <c r="A26" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="23">
         <v>46.1</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="24">
         <v>5.0</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="24">
         <v>99.3</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="24">
         <v>-64.3</v>
       </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="27">
+      <c r="H26" s="27"/>
+      <c r="I26" s="24">
         <v>6.9</v>
       </c>
       <c r="J26" s="14"/>
-      <c r="K26" s="29">
+      <c r="K26" s="26">
         <v>-36.6</v>
       </c>
-      <c r="L26" s="29">
-        <v>-56.5</v>
+      <c r="L26" s="28">
+        <v>6.5</v>
       </c>
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
@@ -2965,9 +3085,15 @@
       <c r="Y26" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z26" s="21"/>
-      <c r="AA26" s="21"/>
-      <c r="AB26" s="21"/>
+      <c r="Z26" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA26" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB26" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC26" s="14"/>
       <c r="AD26" s="17">
         <v>0.0</v>
@@ -2976,10 +3102,10 @@
       <c r="AF26" s="18">
         <v>4.0</v>
       </c>
-      <c r="AG26" s="28">
+      <c r="AG26" s="25">
         <v>0.0</v>
       </c>
-      <c r="AH26" s="28">
+      <c r="AH26" s="25">
         <v>12.0</v>
       </c>
       <c r="AI26" s="3" t="s">
@@ -2989,7 +3115,7 @@
         <v>47</v>
       </c>
       <c r="AK26" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL26" s="3" t="s">
         <v>49</v>
@@ -2998,39 +3124,39 @@
       <c r="AN26" s="3"/>
     </row>
     <row r="27">
-      <c r="A27" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B27" s="23" t="s">
+      <c r="A27" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="23">
         <v>46.1</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="24">
         <v>2.0</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="24">
         <v>143.2</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="24">
         <v>-66.4</v>
       </c>
-      <c r="H27" s="26">
+      <c r="H27" s="23">
         <v>4447.8</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="24">
         <v>3.8</v>
       </c>
       <c r="J27" s="14"/>
-      <c r="K27" s="29">
+      <c r="K27" s="26">
         <v>-65.2</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="26">
         <v>-5.2</v>
       </c>
       <c r="M27" s="14"/>
@@ -3062,9 +3188,15 @@
       <c r="Y27" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z27" s="21"/>
-      <c r="AA27" s="21"/>
-      <c r="AB27" s="21"/>
+      <c r="Z27" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA27" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB27" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC27" s="14"/>
       <c r="AD27" s="17">
         <v>0.0</v>
@@ -3073,10 +3205,10 @@
       <c r="AF27" s="18">
         <v>4.0</v>
       </c>
-      <c r="AG27" s="28">
+      <c r="AG27" s="25">
         <v>0.0</v>
       </c>
-      <c r="AH27" s="28">
+      <c r="AH27" s="25">
         <v>12.0</v>
       </c>
       <c r="AI27" s="3" t="s">
@@ -3086,7 +3218,7 @@
         <v>47</v>
       </c>
       <c r="AK27" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL27" s="3" t="s">
         <v>49</v>
@@ -3095,39 +3227,39 @@
       <c r="AN27" s="3"/>
     </row>
     <row r="28">
-      <c r="A28" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="23" t="s">
+      <c r="A28" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="23">
         <v>46.1</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="23">
         <f t="shared" si="3"/>
         <v>244.9</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="24">
         <v>8.0</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="24">
         <v>161.8</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="24">
         <v>-54.8</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="23">
         <v>599.6</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="24">
         <v>2.3</v>
       </c>
       <c r="J28" s="14"/>
-      <c r="K28" s="29">
+      <c r="K28" s="26">
         <v>-72.6</v>
       </c>
-      <c r="L28" s="29">
+      <c r="L28" s="26">
         <v>-56.8</v>
       </c>
       <c r="M28" s="14"/>
@@ -3159,9 +3291,15 @@
       <c r="Y28" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z28" s="21"/>
-      <c r="AA28" s="21"/>
-      <c r="AB28" s="21"/>
+      <c r="Z28" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA28" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB28" s="17">
+        <v>1.0</v>
+      </c>
       <c r="AC28" s="14"/>
       <c r="AD28" s="17">
         <v>0.0</v>
@@ -3181,7 +3319,7 @@
         <v>47</v>
       </c>
       <c r="AK28" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL28" s="3" t="s">
         <v>49</v>
@@ -3190,38 +3328,38 @@
       <c r="AN28" s="3"/>
     </row>
     <row r="29">
-      <c r="A29" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="23" t="s">
+      <c r="A29" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="24">
         <v>45.8</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="24">
         <v>246.1</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="24">
         <v>7.0</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="24">
         <v>270.1</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="24">
         <v>-71.9</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="24">
         <v>113.4</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="24">
         <v>5.7</v>
       </c>
       <c r="J29" s="14"/>
-      <c r="K29" s="27">
+      <c r="K29" s="24">
         <v>-36.8</v>
       </c>
-      <c r="L29" s="27">
+      <c r="L29" s="24">
         <v>108.3</v>
       </c>
       <c r="M29" s="14"/>
@@ -3253,9 +3391,15 @@
       <c r="Y29" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z29" s="21"/>
-      <c r="AA29" s="21"/>
-      <c r="AB29" s="21"/>
+      <c r="Z29" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA29" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB29" s="18">
+        <v>2.0</v>
+      </c>
       <c r="AC29" s="14"/>
       <c r="AD29" s="17">
         <v>0.0</v>
@@ -3264,7 +3408,7 @@
       <c r="AF29" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG29" s="28">
+      <c r="AG29" s="25">
         <v>2.0</v>
       </c>
       <c r="AH29" s="14"/>
@@ -3275,7 +3419,7 @@
         <v>47</v>
       </c>
       <c r="AK29" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL29" s="3" t="s">
         <v>49</v>
@@ -3284,38 +3428,38 @@
       <c r="AN29" s="3"/>
     </row>
     <row r="30">
-      <c r="A30" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="23" t="s">
+      <c r="A30" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C30" s="24">
         <v>45.9</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D30" s="24">
         <v>246.1</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="24">
         <v>7.0</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="24">
         <v>233.7</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="24">
         <v>-60.3</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30" s="24">
         <v>99.7</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I30" s="24">
         <v>6.1</v>
       </c>
       <c r="J30" s="14"/>
-      <c r="K30" s="27">
+      <c r="K30" s="24">
         <v>-51.5</v>
       </c>
-      <c r="L30" s="27">
+      <c r="L30" s="24">
         <v>142.8</v>
       </c>
       <c r="M30" s="14"/>
@@ -3347,9 +3491,15 @@
       <c r="Y30" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z30" s="21"/>
-      <c r="AA30" s="21"/>
-      <c r="AB30" s="21"/>
+      <c r="Z30" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA30" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB30" s="18">
+        <v>2.0</v>
+      </c>
       <c r="AC30" s="14"/>
       <c r="AD30" s="17">
         <v>0.0</v>
@@ -3358,7 +3508,7 @@
       <c r="AF30" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG30" s="28">
+      <c r="AG30" s="25">
         <v>2.0</v>
       </c>
       <c r="AH30" s="14"/>
@@ -3369,7 +3519,7 @@
         <v>47</v>
       </c>
       <c r="AK30" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL30" s="3" t="s">
         <v>49</v>
@@ -3378,38 +3528,38 @@
       <c r="AN30" s="3"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="23" t="s">
+      <c r="A31" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="24">
         <v>45.9</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="24">
         <v>246.2</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E31" s="24">
         <v>6.0</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="24">
         <v>350.9</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="24">
         <v>67.8</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H31" s="24">
         <v>138.0</v>
       </c>
-      <c r="I31" s="27">
+      <c r="I31" s="24">
         <v>5.7</v>
       </c>
       <c r="J31" s="14"/>
-      <c r="K31" s="27">
+      <c r="K31" s="24">
         <v>82.2</v>
       </c>
-      <c r="L31" s="27">
+      <c r="L31" s="24">
         <v>-161.5</v>
       </c>
       <c r="M31" s="14"/>
@@ -3441,9 +3591,15 @@
       <c r="Y31" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z31" s="21"/>
-      <c r="AA31" s="21"/>
-      <c r="AB31" s="21"/>
+      <c r="Z31" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA31" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB31" s="18">
+        <v>2.0</v>
+      </c>
       <c r="AC31" s="14"/>
       <c r="AD31" s="17">
         <v>0.0</v>
@@ -3452,7 +3608,7 @@
       <c r="AF31" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG31" s="28">
+      <c r="AG31" s="25">
         <v>2.0</v>
       </c>
       <c r="AH31" s="14"/>
@@ -3463,7 +3619,7 @@
         <v>47</v>
       </c>
       <c r="AK31" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL31" s="3" t="s">
         <v>49</v>
@@ -3472,38 +3628,38 @@
       <c r="AN31" s="3"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="23" t="s">
+      <c r="A32" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C32" s="24">
         <v>45.9</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D32" s="24">
         <v>246.3</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="24">
         <v>5.0</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="24">
         <v>100.5</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="24">
         <v>75.0</v>
       </c>
-      <c r="H32" s="27">
+      <c r="H32" s="24">
         <v>142.8</v>
       </c>
-      <c r="I32" s="27">
+      <c r="I32" s="24">
         <v>6.4</v>
       </c>
       <c r="J32" s="14"/>
-      <c r="K32" s="27">
+      <c r="K32" s="24">
         <v>35.3</v>
       </c>
-      <c r="L32" s="27">
+      <c r="L32" s="24">
         <v>-79.8</v>
       </c>
       <c r="M32" s="14"/>
@@ -3535,9 +3691,15 @@
       <c r="Y32" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z32" s="21"/>
-      <c r="AA32" s="21"/>
-      <c r="AB32" s="21"/>
+      <c r="Z32" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA32" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB32" s="18">
+        <v>2.0</v>
+      </c>
       <c r="AC32" s="14"/>
       <c r="AD32" s="17">
         <v>0.0</v>
@@ -3546,7 +3708,7 @@
       <c r="AF32" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG32" s="28">
+      <c r="AG32" s="25">
         <v>2.0</v>
       </c>
       <c r="AH32" s="14"/>
@@ -3557,7 +3719,7 @@
         <v>47</v>
       </c>
       <c r="AK32" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL32" s="3" t="s">
         <v>49</v>
@@ -3566,38 +3728,38 @@
       <c r="AN32" s="3"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="23" t="s">
+      <c r="A33" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="24">
         <v>45.9</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="24">
         <v>246.2</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="24">
         <v>6.0</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="24">
         <v>90.6</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="24">
         <v>79.1</v>
       </c>
-      <c r="H33" s="27">
+      <c r="H33" s="24">
         <v>247.3</v>
       </c>
-      <c r="I33" s="27">
+      <c r="I33" s="24">
         <v>4.3</v>
       </c>
       <c r="J33" s="14"/>
-      <c r="K33" s="27">
+      <c r="K33" s="24">
         <v>41.8</v>
       </c>
-      <c r="L33" s="27">
+      <c r="L33" s="24">
         <v>-84.8</v>
       </c>
       <c r="M33" s="14"/>
@@ -3629,9 +3791,15 @@
       <c r="Y33" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z33" s="21"/>
-      <c r="AA33" s="21"/>
-      <c r="AB33" s="21"/>
+      <c r="Z33" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA33" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB33" s="18">
+        <v>2.0</v>
+      </c>
       <c r="AC33" s="14"/>
       <c r="AD33" s="17">
         <v>0.0</v>
@@ -3640,7 +3808,7 @@
       <c r="AF33" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG33" s="28">
+      <c r="AG33" s="25">
         <v>2.0</v>
       </c>
       <c r="AH33" s="14"/>
@@ -3651,7 +3819,7 @@
         <v>47</v>
       </c>
       <c r="AK33" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL33" s="3" t="s">
         <v>49</v>
@@ -3660,38 +3828,38 @@
       <c r="AN33" s="3"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="23" t="s">
+      <c r="A34" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C34" s="24">
         <v>45.9</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D34" s="24">
         <v>246.2</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="24">
         <v>5.0</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="24">
         <v>197.2</v>
       </c>
-      <c r="G34" s="27">
+      <c r="G34" s="24">
         <v>-54.5</v>
       </c>
-      <c r="H34" s="27">
+      <c r="H34" s="24">
         <v>49.5</v>
       </c>
-      <c r="I34" s="27">
+      <c r="I34" s="24">
         <v>11.0</v>
       </c>
       <c r="J34" s="14"/>
-      <c r="K34" s="27">
+      <c r="K34" s="24">
         <v>-73.3</v>
       </c>
-      <c r="L34" s="27">
+      <c r="L34" s="24">
         <v>-170.6</v>
       </c>
       <c r="M34" s="14"/>
@@ -3723,9 +3891,15 @@
       <c r="Y34" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z34" s="21"/>
-      <c r="AA34" s="21"/>
-      <c r="AB34" s="21"/>
+      <c r="Z34" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA34" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB34" s="18">
+        <v>2.0</v>
+      </c>
       <c r="AC34" s="14"/>
       <c r="AD34" s="17">
         <v>0.0</v>
@@ -3734,7 +3908,7 @@
       <c r="AF34" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG34" s="28">
+      <c r="AG34" s="25">
         <v>2.0</v>
       </c>
       <c r="AH34" s="14"/>
@@ -3745,7 +3919,7 @@
         <v>47</v>
       </c>
       <c r="AK34" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL34" s="3" t="s">
         <v>49</v>
@@ -3754,38 +3928,38 @@
       <c r="AN34" s="3"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" s="23" t="s">
+      <c r="A35" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="24">
         <v>46.1</v>
       </c>
-      <c r="D35" s="27">
+      <c r="D35" s="24">
         <v>246.0</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="24">
         <v>3.0</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="24">
         <v>186.2</v>
       </c>
-      <c r="G35" s="27">
+      <c r="G35" s="24">
         <v>-64.1</v>
       </c>
-      <c r="H35" s="27">
+      <c r="H35" s="24">
         <v>78.2</v>
       </c>
-      <c r="I35" s="27">
+      <c r="I35" s="24">
         <v>14.0</v>
       </c>
       <c r="J35" s="14"/>
-      <c r="K35" s="27">
+      <c r="K35" s="24">
         <v>-86.1</v>
       </c>
-      <c r="L35" s="27">
+      <c r="L35" s="24">
         <v>154.8</v>
       </c>
       <c r="M35" s="14"/>
@@ -3817,9 +3991,15 @@
       <c r="Y35" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z35" s="21"/>
-      <c r="AA35" s="21"/>
-      <c r="AB35" s="21"/>
+      <c r="Z35" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA35" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB35" s="18">
+        <v>2.0</v>
+      </c>
       <c r="AC35" s="14"/>
       <c r="AD35" s="17">
         <v>0.0</v>
@@ -3828,7 +4008,7 @@
       <c r="AF35" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG35" s="28">
+      <c r="AG35" s="25">
         <v>2.0</v>
       </c>
       <c r="AH35" s="14"/>
@@ -3839,7 +4019,7 @@
         <v>47</v>
       </c>
       <c r="AK35" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL35" s="3" t="s">
         <v>49</v>
@@ -3848,39 +4028,39 @@
       <c r="AN35" s="3"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B36" s="23" t="s">
+      <c r="A36" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C36" s="24">
         <v>46.1</v>
       </c>
-      <c r="D36" s="27">
+      <c r="D36" s="24">
         <v>246.0</v>
       </c>
-      <c r="E36" s="27">
+      <c r="E36" s="24">
         <v>6.0</v>
       </c>
-      <c r="F36" s="27">
+      <c r="F36" s="24">
         <v>247.8</v>
       </c>
       <c r="G36" s="12">
         <v>-44.9</v>
       </c>
-      <c r="H36" s="27">
+      <c r="H36" s="24">
         <v>596.3</v>
       </c>
-      <c r="I36" s="27">
+      <c r="I36" s="24">
         <v>2.8</v>
       </c>
       <c r="J36" s="14"/>
-      <c r="K36" s="27">
+      <c r="K36" s="24">
         <v>-33.8</v>
       </c>
-      <c r="L36" s="27">
-        <v>-19.5</v>
+      <c r="L36" s="12">
+        <v>151.5</v>
       </c>
       <c r="M36" s="14"/>
       <c r="N36" s="14"/>
@@ -3911,9 +4091,15 @@
       <c r="Y36" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Z36" s="21"/>
-      <c r="AA36" s="21"/>
-      <c r="AB36" s="21"/>
+      <c r="Z36" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA36" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="AB36" s="18">
+        <v>2.0</v>
+      </c>
       <c r="AC36" s="14"/>
       <c r="AD36" s="17">
         <v>0.0</v>
@@ -3922,7 +4108,7 @@
       <c r="AF36" s="17">
         <v>0.0</v>
       </c>
-      <c r="AG36" s="28">
+      <c r="AG36" s="25">
         <v>2.0</v>
       </c>
       <c r="AH36" s="14"/>
@@ -3933,7 +4119,7 @@
         <v>47</v>
       </c>
       <c r="AK36" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL36" s="3" t="s">
         <v>49</v>
@@ -3978,19 +4164,19 @@
       <c r="AM37" s="3"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="23"/>
+      <c r="B38" s="20"/>
       <c r="M38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="31"/>
-      <c r="R38" s="32"/>
-      <c r="S38" s="32"/>
-      <c r="T38" s="32"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
       <c r="W38" s="17"/>
-      <c r="X38" s="33"/>
+      <c r="X38" s="31"/>
       <c r="Y38" s="3"/>
-      <c r="Z38" s="34"/>
+      <c r="Z38" s="32"/>
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
       <c r="AC38" s="3"/>

</xml_diff>